<commit_message>
First attempt at adding multiple devices
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/DevicesData.xlsx
+++ b/src/test/resources/configs/data/excel/DevicesData.xlsx
@@ -9061,8 +9061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I22" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14167,7 +14167,7 @@
         <v>415</v>
       </c>
       <c r="C87" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D87" s="144" t="s">
         <v>137</v>
@@ -14226,7 +14226,7 @@
         <v>415</v>
       </c>
       <c r="C88" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D88" s="144" t="s">
         <v>139</v>
@@ -14285,7 +14285,7 @@
         <v>415</v>
       </c>
       <c r="C89" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D89" s="143" t="s">
         <v>519</v>
@@ -14344,7 +14344,7 @@
         <v>415</v>
       </c>
       <c r="C90" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D90" s="144" t="s">
         <v>521</v>
@@ -14403,7 +14403,7 @@
         <v>415</v>
       </c>
       <c r="C91" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D91" s="144" t="s">
         <v>145</v>
@@ -14462,7 +14462,7 @@
         <v>415</v>
       </c>
       <c r="C92" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D92" s="144" t="s">
         <v>524</v>
@@ -14521,7 +14521,7 @@
         <v>415</v>
       </c>
       <c r="C93" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D93" s="143" t="s">
         <v>149</v>
@@ -14580,7 +14580,7 @@
         <v>415</v>
       </c>
       <c r="C94" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D94" s="144" t="s">
         <v>527</v>
@@ -14639,7 +14639,7 @@
         <v>415</v>
       </c>
       <c r="C95" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D95" s="144" t="s">
         <v>528</v>
@@ -14698,7 +14698,7 @@
         <v>415</v>
       </c>
       <c r="C96" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D96" s="144" t="s">
         <v>530</v>
@@ -14757,7 +14757,7 @@
         <v>415</v>
       </c>
       <c r="C97" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D97" s="143" t="s">
         <v>532</v>
@@ -14816,7 +14816,7 @@
         <v>415</v>
       </c>
       <c r="C98" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D98" s="144" t="s">
         <v>534</v>
@@ -14875,7 +14875,7 @@
         <v>415</v>
       </c>
       <c r="C99" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D99" s="144" t="s">
         <v>536</v>
@@ -14934,7 +14934,7 @@
         <v>415</v>
       </c>
       <c r="C100" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D100" s="144" t="s">
         <v>163</v>
@@ -14993,7 +14993,7 @@
         <v>415</v>
       </c>
       <c r="C101" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D101" s="143" t="s">
         <v>165</v>
@@ -15052,7 +15052,7 @@
         <v>415</v>
       </c>
       <c r="C102" s="147" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D102" s="144" t="s">
         <v>540</v>

</xml_diff>

<commit_message>
Add devices in a loop
Upto 100 devices, still testing this
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/DevicesData.xlsx
+++ b/src/test/resources/configs/data/excel/DevicesData.xlsx
@@ -3178,7 +3178,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z137"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -9061,8 +9061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12096,7 +12096,7 @@
     </row>
     <row r="52" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="148" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B52" s="145" t="s">
         <v>22</v>
@@ -13335,7 +13335,7 @@
     </row>
     <row r="73" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B73" s="147" t="s">
         <v>415</v>
@@ -13571,7 +13571,7 @@
     </row>
     <row r="77" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B77" s="147" t="s">
         <v>415</v>
@@ -13807,7 +13807,7 @@
     </row>
     <row r="81" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B81" s="147" t="s">
         <v>415</v>
@@ -14043,7 +14043,7 @@
     </row>
     <row r="85" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B85" s="147" t="s">
         <v>415</v>
@@ -14279,7 +14279,7 @@
     </row>
     <row r="89" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B89" s="147" t="s">
         <v>415</v>
@@ -14515,7 +14515,7 @@
     </row>
     <row r="93" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B93" s="147" t="s">
         <v>415</v>
@@ -14751,7 +14751,7 @@
     </row>
     <row r="97" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B97" s="147" t="s">
         <v>415</v>
@@ -14987,7 +14987,7 @@
     </row>
     <row r="101" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B101" s="147" t="s">
         <v>415</v>
@@ -15223,7 +15223,7 @@
     </row>
     <row r="105" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B105" s="147" t="s">
         <v>415</v>
@@ -15459,7 +15459,7 @@
     </row>
     <row r="109" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B109" s="147" t="s">
         <v>415</v>
@@ -15695,7 +15695,7 @@
     </row>
     <row r="113" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B113" s="147" t="s">
         <v>415</v>
@@ -15931,7 +15931,7 @@
     </row>
     <row r="117" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B117" s="147" t="s">
         <v>415</v>
@@ -16167,7 +16167,7 @@
     </row>
     <row r="121" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B121" s="147" t="s">
         <v>415</v>
@@ -16403,7 +16403,7 @@
     </row>
     <row r="125" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B125" s="147" t="s">
         <v>415</v>
@@ -16639,7 +16639,7 @@
     </row>
     <row r="129" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B129" s="147" t="s">
         <v>415</v>
@@ -16875,7 +16875,7 @@
     </row>
     <row r="133" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B133" s="147" t="s">
         <v>415</v>
@@ -17053,7 +17053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y146"/>
   <sheetViews>
-    <sheetView topLeftCell="O24" workbookViewId="0">
+    <sheetView topLeftCell="A127" workbookViewId="0">
       <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed failing smoke tests
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/DevicesData.xlsx
+++ b/src/test/resources/configs/data/excel/DevicesData.xlsx
@@ -3167,7 +3167,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8159,33 +8159,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="Control 1">
+        <control shapeId="1027" r:id="rId4" name="Control 3">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+        <control shapeId="1027" r:id="rId4" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1026" r:id="rId6" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId7">
+          <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
@@ -8209,27 +8209,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId8" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId7">
+        <control shapeId="1025" r:id="rId7" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId8" name="Control 3"/>
+        <control shapeId="1025" r:id="rId7" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9061,7 +9061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed tests not related to Adding Devices
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/DevicesData.xlsx
+++ b/src/test/resources/configs/data/excel/DevicesData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6686" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6724" uniqueCount="616">
   <si>
     <t>GMD (C-Y)</t>
   </si>
@@ -3167,7 +3167,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8159,33 +8159,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId4" name="Control 3">
+        <control shapeId="1025" r:id="rId4" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId4" name="Control 3"/>
+        <control shapeId="1025" r:id="rId4" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1026" r:id="rId6" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId5">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
@@ -8209,27 +8209,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId7" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId8">
+        <control shapeId="1027" r:id="rId8" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId7" name="Control 1"/>
+        <control shapeId="1027" r:id="rId8" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8705,7 +8705,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -8758,7 +8758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -8787,7 +8787,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -8840,7 +8840,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -8893,7 +8893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -9062,7 +9062,7 @@
   <dimension ref="A1:S146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9146,7 +9146,7 @@
     </row>
     <row r="2" spans="1:19" s="148" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="148" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="149" t="s">
         <v>399</v>
@@ -16992,12 +16992,122 @@
       </c>
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N135" s="99"/>
-      <c r="O135" s="99"/>
-    </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N136" s="99"/>
-      <c r="O136" s="99"/>
+      <c r="A135" s="168" t="s">
+        <v>416</v>
+      </c>
+      <c r="B135" s="168" t="s">
+        <v>30</v>
+      </c>
+      <c r="C135" s="168" t="s">
+        <v>412</v>
+      </c>
+      <c r="D135" s="169" t="s">
+        <v>283</v>
+      </c>
+      <c r="E135" s="169" t="s">
+        <v>284</v>
+      </c>
+      <c r="F135" s="170" t="s">
+        <v>1</v>
+      </c>
+      <c r="G135" s="171" t="s">
+        <v>413</v>
+      </c>
+      <c r="H135" s="168" t="s">
+        <v>2</v>
+      </c>
+      <c r="I135" s="171" t="s">
+        <v>13</v>
+      </c>
+      <c r="J135" s="171" t="s">
+        <v>285</v>
+      </c>
+      <c r="K135" s="168" t="s">
+        <v>15</v>
+      </c>
+      <c r="L135" s="170" t="s">
+        <v>26</v>
+      </c>
+      <c r="M135" s="168" t="s">
+        <v>27</v>
+      </c>
+      <c r="N135" s="169" t="s">
+        <v>292</v>
+      </c>
+      <c r="O135" s="171" t="s">
+        <v>608</v>
+      </c>
+      <c r="P135" s="169" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q135" s="171" t="s">
+        <v>386</v>
+      </c>
+      <c r="R135" s="171" t="s">
+        <v>396</v>
+      </c>
+      <c r="S135" s="168" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" s="148" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="148" t="s">
+        <v>16</v>
+      </c>
+      <c r="B136" s="149" t="s">
+        <v>399</v>
+      </c>
+      <c r="C136" s="149" t="s">
+        <v>433</v>
+      </c>
+      <c r="D136" s="143" t="s">
+        <v>38</v>
+      </c>
+      <c r="E136" s="143" t="s">
+        <v>434</v>
+      </c>
+      <c r="F136" s="172" t="s">
+        <v>16</v>
+      </c>
+      <c r="G136" s="172" t="s">
+        <v>16</v>
+      </c>
+      <c r="H136" s="172" t="s">
+        <v>17</v>
+      </c>
+      <c r="I136" s="149" t="s">
+        <v>433</v>
+      </c>
+      <c r="J136" s="149" t="s">
+        <v>433</v>
+      </c>
+      <c r="K136" s="149" t="s">
+        <v>433</v>
+      </c>
+      <c r="L136" s="149" t="s">
+        <v>433</v>
+      </c>
+      <c r="M136" s="149" t="s">
+        <v>433</v>
+      </c>
+      <c r="N136" s="149" t="s">
+        <v>433</v>
+      </c>
+      <c r="O136" s="149" t="s">
+        <v>433</v>
+      </c>
+      <c r="P136" s="149" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q136" s="149" t="s">
+        <v>433</v>
+      </c>
+      <c r="R136" s="149" t="s">
+        <v>433</v>
+      </c>
+      <c r="S136" s="149" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B141" s="177" t="s">

</xml_diff>

<commit_message>
Added 1 class to add devices - Multiple user - Multiple device types
It takes around 15 mins per user
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/DevicesData.xlsx
+++ b/src/test/resources/configs/data/excel/DevicesData.xlsx
@@ -3167,7 +3167,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8159,33 +8159,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId4" name="Control 3">
+        <control shapeId="1025" r:id="rId4" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId4" name="Control 3"/>
+        <control shapeId="1025" r:id="rId4" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1026" r:id="rId6" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId5">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
@@ -8209,27 +8209,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId7" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId8">
+        <control shapeId="1027" r:id="rId8" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId7" name="Control 1"/>
+        <control shapeId="1027" r:id="rId8" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9061,8 +9061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10561,8 +10561,8 @@
       </c>
     </row>
     <row r="26" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="148" t="s">
-        <v>16</v>
+      <c r="A26" s="146" t="s">
+        <v>17</v>
       </c>
       <c r="B26" s="173" t="s">
         <v>401</v>
@@ -11564,8 +11564,8 @@
       </c>
     </row>
     <row r="43" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="148" t="s">
-        <v>16</v>
+      <c r="A43" s="146" t="s">
+        <v>17</v>
       </c>
       <c r="B43" s="173" t="s">
         <v>401</v>
@@ -12096,7 +12096,7 @@
     </row>
     <row r="52" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B52" s="145" t="s">
         <v>22</v>
@@ -13335,7 +13335,7 @@
     </row>
     <row r="73" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B73" s="147" t="s">
         <v>415</v>
@@ -13571,7 +13571,7 @@
     </row>
     <row r="77" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B77" s="147" t="s">
         <v>415</v>
@@ -16874,8 +16874,8 @@
       </c>
     </row>
     <row r="133" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="148" t="s">
-        <v>16</v>
+      <c r="A133" s="146" t="s">
+        <v>17</v>
       </c>
       <c r="B133" s="147" t="s">
         <v>415</v>

</xml_diff>

<commit_message>
New code changes introduced:
	- Tests failing due to the new push
		- Its removed the gmdn buttons and the way we add new devices
		- Also the work flow of some of the pages
			- Now we have to declare device types first and than create new organisations
			- Adding devices no longer have to select radio button to specify gmdn definition or term
			- Auto suggestion removed, now it displays a match below the gmdn box
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/DevicesData.xlsx
+++ b/src/test/resources/configs/data/excel/DevicesData.xlsx
@@ -2666,6 +2666,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2719,9 +2722,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3176,7 +3176,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3301,7 +3301,7 @@
       <c r="Z2" s="132"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="184" t="s">
+      <c r="A3" s="185" t="s">
         <v>410</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -3338,7 +3338,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="185"/>
+      <c r="A4" s="186"/>
       <c r="B4" s="61" t="s">
         <v>40</v>
       </c>
@@ -3373,7 +3373,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="185"/>
+      <c r="A5" s="186"/>
       <c r="B5" s="61" t="s">
         <v>42</v>
       </c>
@@ -3408,7 +3408,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="186"/>
+      <c r="A6" s="187"/>
       <c r="B6" s="70" t="s">
         <v>44</v>
       </c>
@@ -3474,7 +3474,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="181" t="s">
+      <c r="A8" s="182" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -3513,7 +3513,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="182"/>
+      <c r="A9" s="183"/>
       <c r="B9" s="10" t="s">
         <v>48</v>
       </c>
@@ -3544,7 +3544,7 @@
       <c r="S9" s="8"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="182"/>
+      <c r="A10" s="183"/>
       <c r="B10" s="10" t="s">
         <v>50</v>
       </c>
@@ -3575,7 +3575,7 @@
       <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="183"/>
+      <c r="A11" s="184"/>
       <c r="B11" s="13" t="s">
         <v>52</v>
       </c>
@@ -3604,7 +3604,7 @@
       <c r="S11" s="23"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="187" t="s">
+      <c r="A12" s="188" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="54" t="s">
@@ -3637,7 +3637,7 @@
       <c r="S12" s="59"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="188"/>
+      <c r="A13" s="189"/>
       <c r="B13" s="61" t="s">
         <v>56</v>
       </c>
@@ -3669,7 +3669,7 @@
       <c r="Z13" s="22"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="188"/>
+      <c r="A14" s="189"/>
       <c r="B14" s="61" t="s">
         <v>58</v>
       </c>
@@ -3700,7 +3700,7 @@
       <c r="S14" s="59"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="189"/>
+      <c r="A15" s="190"/>
       <c r="B15" s="65" t="s">
         <v>60</v>
       </c>
@@ -3729,7 +3729,7 @@
       <c r="S15" s="87"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="187" t="s">
+      <c r="A16" s="188" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="54" t="s">
@@ -3762,7 +3762,7 @@
       <c r="S16" s="59"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="188"/>
+      <c r="A17" s="189"/>
       <c r="B17" s="61" t="s">
         <v>63</v>
       </c>
@@ -3793,7 +3793,7 @@
       <c r="S17" s="59"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="188"/>
+      <c r="A18" s="189"/>
       <c r="B18" s="61" t="s">
         <v>65</v>
       </c>
@@ -3824,7 +3824,7 @@
       <c r="S18" s="59"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="189"/>
+      <c r="A19" s="190"/>
       <c r="B19" s="65" t="s">
         <v>67</v>
       </c>
@@ -3853,7 +3853,7 @@
       <c r="S19" s="87"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="188" t="s">
+      <c r="A20" s="189" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="61" t="s">
@@ -3886,7 +3886,7 @@
       <c r="S20" s="59"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="188"/>
+      <c r="A21" s="189"/>
       <c r="B21" s="61" t="s">
         <v>71</v>
       </c>
@@ -3917,7 +3917,7 @@
       <c r="S21" s="59"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="188"/>
+      <c r="A22" s="189"/>
       <c r="B22" s="61" t="s">
         <v>73</v>
       </c>
@@ -3948,7 +3948,7 @@
       <c r="S22" s="59"/>
     </row>
     <row r="23" spans="1:19" s="27" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="190"/>
+      <c r="A23" s="191"/>
       <c r="B23" s="70" t="s">
         <v>75</v>
       </c>
@@ -4018,7 +4018,7 @@
       <c r="S24" s="52"/>
     </row>
     <row r="25" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="191" t="s">
+      <c r="A25" s="192" t="s">
         <v>286</v>
       </c>
       <c r="B25" s="25" t="s">
@@ -4063,7 +4063,7 @@
       <c r="S25" s="8"/>
     </row>
     <row r="26" spans="1:19" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="179"/>
+      <c r="A26" s="180"/>
       <c r="B26" s="10" t="s">
         <v>237</v>
       </c>
@@ -4104,7 +4104,7 @@
       <c r="S26" s="8"/>
     </row>
     <row r="27" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="179"/>
+      <c r="A27" s="180"/>
       <c r="B27" s="10" t="s">
         <v>239</v>
       </c>
@@ -4149,7 +4149,7 @@
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="179"/>
+      <c r="A28" s="180"/>
       <c r="B28" s="10" t="s">
         <v>241</v>
       </c>
@@ -4192,7 +4192,7 @@
       <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="179"/>
+      <c r="A29" s="180"/>
       <c r="B29" s="10" t="s">
         <v>243</v>
       </c>
@@ -4231,7 +4231,7 @@
       <c r="S29" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="179"/>
+      <c r="A30" s="180"/>
       <c r="B30" s="10" t="s">
         <v>245</v>
       </c>
@@ -4274,7 +4274,7 @@
       <c r="S30" s="8"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="179"/>
+      <c r="A31" s="180"/>
       <c r="B31" s="10" t="s">
         <v>247</v>
       </c>
@@ -4317,7 +4317,7 @@
       <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="192"/>
+      <c r="A32" s="193"/>
       <c r="B32" s="13" t="s">
         <v>249</v>
       </c>
@@ -4360,7 +4360,7 @@
       <c r="S32" s="23"/>
     </row>
     <row r="33" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="178" t="s">
+      <c r="A33" s="179" t="s">
         <v>287</v>
       </c>
       <c r="B33" s="15" t="s">
@@ -4407,7 +4407,7 @@
       <c r="S33" s="8"/>
     </row>
     <row r="34" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="179"/>
+      <c r="A34" s="180"/>
       <c r="B34" s="10" t="s">
         <v>253</v>
       </c>
@@ -4450,7 +4450,7 @@
       <c r="S34" s="8"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35" s="179"/>
+      <c r="A35" s="180"/>
       <c r="B35" s="10" t="s">
         <v>255</v>
       </c>
@@ -4489,7 +4489,7 @@
       <c r="S35" s="8"/>
     </row>
     <row r="36" spans="1:22" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="179"/>
+      <c r="A36" s="180"/>
       <c r="B36" s="10" t="s">
         <v>257</v>
       </c>
@@ -4532,7 +4532,7 @@
       <c r="S36" s="8"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="179"/>
+      <c r="A37" s="180"/>
       <c r="B37" s="10" t="s">
         <v>259</v>
       </c>
@@ -4577,7 +4577,7 @@
       <c r="S37" s="8"/>
     </row>
     <row r="38" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="179"/>
+      <c r="A38" s="180"/>
       <c r="B38" s="10" t="s">
         <v>261</v>
       </c>
@@ -4620,7 +4620,7 @@
       <c r="S38" s="8"/>
     </row>
     <row r="39" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="179"/>
+      <c r="A39" s="180"/>
       <c r="B39" s="10" t="s">
         <v>263</v>
       </c>
@@ -4665,7 +4665,7 @@
       <c r="S39" s="8"/>
     </row>
     <row r="40" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="192"/>
+      <c r="A40" s="193"/>
       <c r="B40" s="13" t="s">
         <v>265</v>
       </c>
@@ -4708,7 +4708,7 @@
       <c r="S40" s="23"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="178" t="s">
+      <c r="A41" s="179" t="s">
         <v>288</v>
       </c>
       <c r="B41" s="15" t="s">
@@ -4749,7 +4749,7 @@
       <c r="S41" s="8"/>
     </row>
     <row r="42" spans="1:22" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="179"/>
+      <c r="A42" s="180"/>
       <c r="B42" s="10" t="s">
         <v>269</v>
       </c>
@@ -4792,7 +4792,7 @@
       <c r="S42" s="8"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="179"/>
+      <c r="A43" s="180"/>
       <c r="B43" s="10" t="s">
         <v>270</v>
       </c>
@@ -4837,7 +4837,7 @@
       <c r="S43" s="8"/>
     </row>
     <row r="44" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="179"/>
+      <c r="A44" s="180"/>
       <c r="B44" s="10" t="s">
         <v>272</v>
       </c>
@@ -4880,7 +4880,7 @@
       <c r="S44" s="8"/>
     </row>
     <row r="45" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="179"/>
+      <c r="A45" s="180"/>
       <c r="B45" s="10" t="s">
         <v>274</v>
       </c>
@@ -4925,7 +4925,7 @@
       <c r="S45" s="8"/>
     </row>
     <row r="46" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="179"/>
+      <c r="A46" s="180"/>
       <c r="B46" s="10" t="s">
         <v>276</v>
       </c>
@@ -4968,7 +4968,7 @@
       <c r="S46" s="8"/>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47" s="179"/>
+      <c r="A47" s="180"/>
       <c r="B47" s="10" t="s">
         <v>278</v>
       </c>
@@ -5007,7 +5007,7 @@
       <c r="S47" s="8"/>
     </row>
     <row r="48" spans="1:22" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="180"/>
+      <c r="A48" s="181"/>
       <c r="B48" s="11" t="s">
         <v>280</v>
       </c>
@@ -5230,7 +5230,7 @@
       <c r="S54" s="52"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A55" s="193" t="s">
+      <c r="A55" s="194" t="s">
         <v>411</v>
       </c>
       <c r="B55" s="61" t="s">
@@ -5269,7 +5269,7 @@
       <c r="S55" s="59"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A56" s="194"/>
+      <c r="A56" s="195"/>
       <c r="B56" s="61" t="s">
         <v>87</v>
       </c>
@@ -5306,7 +5306,7 @@
       <c r="S56" s="59"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A57" s="194"/>
+      <c r="A57" s="195"/>
       <c r="B57" s="134" t="s">
         <v>89</v>
       </c>
@@ -5343,7 +5343,7 @@
       <c r="S57" s="140"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A58" s="194"/>
+      <c r="A58" s="195"/>
       <c r="B58" s="61" t="s">
         <v>91</v>
       </c>
@@ -5380,7 +5380,7 @@
       <c r="S58" s="59"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A59" s="194"/>
+      <c r="A59" s="195"/>
       <c r="B59" s="61" t="s">
         <v>93</v>
       </c>
@@ -5417,7 +5417,7 @@
       <c r="S59" s="59"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A60" s="194"/>
+      <c r="A60" s="195"/>
       <c r="B60" s="61" t="s">
         <v>95</v>
       </c>
@@ -5454,7 +5454,7 @@
       <c r="S60" s="59"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A61" s="194"/>
+      <c r="A61" s="195"/>
       <c r="B61" s="134" t="s">
         <v>97</v>
       </c>
@@ -5491,7 +5491,7 @@
       <c r="S61" s="140"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A62" s="194"/>
+      <c r="A62" s="195"/>
       <c r="B62" s="61" t="s">
         <v>99</v>
       </c>
@@ -5528,7 +5528,7 @@
       <c r="S62" s="59"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A63" s="194"/>
+      <c r="A63" s="195"/>
       <c r="B63" s="61" t="s">
         <v>103</v>
       </c>
@@ -5565,7 +5565,7 @@
       <c r="S63" s="59"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A64" s="194"/>
+      <c r="A64" s="195"/>
       <c r="B64" s="61" t="s">
         <v>105</v>
       </c>
@@ -5602,7 +5602,7 @@
       <c r="S64" s="59"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A65" s="194"/>
+      <c r="A65" s="195"/>
       <c r="B65" s="134" t="s">
         <v>113</v>
       </c>
@@ -5639,7 +5639,7 @@
       <c r="S65" s="140"/>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A66" s="194"/>
+      <c r="A66" s="195"/>
       <c r="B66" s="61" t="s">
         <v>115</v>
       </c>
@@ -5676,7 +5676,7 @@
       <c r="S66" s="59"/>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A67" s="194"/>
+      <c r="A67" s="195"/>
       <c r="B67" s="61" t="s">
         <v>119</v>
       </c>
@@ -5713,7 +5713,7 @@
       <c r="S67" s="59"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A68" s="194"/>
+      <c r="A68" s="195"/>
       <c r="B68" s="61" t="s">
         <v>36</v>
       </c>
@@ -5748,7 +5748,7 @@
       <c r="S68" s="59"/>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A69" s="194"/>
+      <c r="A69" s="195"/>
       <c r="B69" s="134" t="s">
         <v>125</v>
       </c>
@@ -5783,7 +5783,7 @@
       <c r="S69" s="140"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="195"/>
+      <c r="A70" s="196"/>
       <c r="B70" s="70" t="s">
         <v>127</v>
       </c>
@@ -5851,7 +5851,7 @@
       <c r="S71" s="52"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A72" s="191" t="s">
+      <c r="A72" s="192" t="s">
         <v>4</v>
       </c>
       <c r="B72" s="82" t="s">
@@ -5890,7 +5890,7 @@
       <c r="S72" s="59"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A73" s="179"/>
+      <c r="A73" s="180"/>
       <c r="B73" s="61" t="s">
         <v>79</v>
       </c>
@@ -5927,7 +5927,7 @@
       <c r="S73" s="59"/>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A74" s="179"/>
+      <c r="A74" s="180"/>
       <c r="B74" s="10" t="s">
         <v>81</v>
       </c>
@@ -5964,7 +5964,7 @@
       <c r="S74" s="8"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A75" s="179"/>
+      <c r="A75" s="180"/>
       <c r="B75" s="61" t="s">
         <v>101</v>
       </c>
@@ -6001,7 +6001,7 @@
       <c r="S75" s="59"/>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A76" s="179"/>
+      <c r="A76" s="180"/>
       <c r="B76" s="61" t="s">
         <v>107</v>
       </c>
@@ -6038,7 +6038,7 @@
       <c r="S76" s="59"/>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A77" s="179"/>
+      <c r="A77" s="180"/>
       <c r="B77" s="61" t="s">
         <v>32</v>
       </c>
@@ -6075,7 +6075,7 @@
       <c r="S77" s="59"/>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A78" s="179"/>
+      <c r="A78" s="180"/>
       <c r="B78" s="10" t="s">
         <v>34</v>
       </c>
@@ -6112,7 +6112,7 @@
       <c r="S78" s="8"/>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A79" s="179"/>
+      <c r="A79" s="180"/>
       <c r="B79" s="61" t="s">
         <v>109</v>
       </c>
@@ -6149,7 +6149,7 @@
       <c r="S79" s="59"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A80" s="179"/>
+      <c r="A80" s="180"/>
       <c r="B80" s="61" t="s">
         <v>111</v>
       </c>
@@ -6186,7 +6186,7 @@
       <c r="S80" s="59"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A81" s="179"/>
+      <c r="A81" s="180"/>
       <c r="B81" s="61" t="s">
         <v>117</v>
       </c>
@@ -6223,7 +6223,7 @@
       <c r="S81" s="59"/>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A82" s="179"/>
+      <c r="A82" s="180"/>
       <c r="B82" s="10" t="s">
         <v>121</v>
       </c>
@@ -6260,7 +6260,7 @@
       <c r="S82" s="8"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A83" s="179"/>
+      <c r="A83" s="180"/>
       <c r="B83" s="61" t="s">
         <v>123</v>
       </c>
@@ -6297,7 +6297,7 @@
       <c r="S83" s="59"/>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A84" s="179"/>
+      <c r="A84" s="180"/>
       <c r="B84" s="61" t="s">
         <v>129</v>
       </c>
@@ -6332,7 +6332,7 @@
       <c r="S84" s="59"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A85" s="179"/>
+      <c r="A85" s="180"/>
       <c r="B85" s="61" t="s">
         <v>131</v>
       </c>
@@ -6367,7 +6367,7 @@
       <c r="S85" s="59"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A86" s="179"/>
+      <c r="A86" s="180"/>
       <c r="B86" s="10" t="s">
         <v>133</v>
       </c>
@@ -6401,7 +6401,7 @@
       <c r="S86" s="8"/>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A87" s="192"/>
+      <c r="A87" s="193"/>
       <c r="B87" s="65" t="s">
         <v>135</v>
       </c>
@@ -6436,7 +6436,7 @@
       <c r="S87" s="87"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A88" s="178" t="s">
+      <c r="A88" s="179" t="s">
         <v>5</v>
       </c>
       <c r="B88" s="54" t="s">
@@ -6475,7 +6475,7 @@
       <c r="S88" s="59"/>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A89" s="179"/>
+      <c r="A89" s="180"/>
       <c r="B89" s="61" t="s">
         <v>139</v>
       </c>
@@ -6512,7 +6512,7 @@
       <c r="S89" s="59"/>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A90" s="179"/>
+      <c r="A90" s="180"/>
       <c r="B90" s="10" t="s">
         <v>141</v>
       </c>
@@ -6549,7 +6549,7 @@
       <c r="S90" s="8"/>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A91" s="179"/>
+      <c r="A91" s="180"/>
       <c r="B91" s="61" t="s">
         <v>143</v>
       </c>
@@ -6586,7 +6586,7 @@
       <c r="S91" s="59"/>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A92" s="179"/>
+      <c r="A92" s="180"/>
       <c r="B92" s="61" t="s">
         <v>145</v>
       </c>
@@ -6623,7 +6623,7 @@
       <c r="S92" s="59"/>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A93" s="179"/>
+      <c r="A93" s="180"/>
       <c r="B93" s="61" t="s">
         <v>147</v>
       </c>
@@ -6660,7 +6660,7 @@
       <c r="S93" s="59"/>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A94" s="179"/>
+      <c r="A94" s="180"/>
       <c r="B94" s="10" t="s">
         <v>149</v>
       </c>
@@ -6697,7 +6697,7 @@
       <c r="S94" s="8"/>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A95" s="179"/>
+      <c r="A95" s="180"/>
       <c r="B95" s="61" t="s">
         <v>151</v>
       </c>
@@ -6734,7 +6734,7 @@
       <c r="S95" s="59"/>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A96" s="179"/>
+      <c r="A96" s="180"/>
       <c r="B96" s="61" t="s">
         <v>153</v>
       </c>
@@ -6771,7 +6771,7 @@
       <c r="S96" s="59"/>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A97" s="179"/>
+      <c r="A97" s="180"/>
       <c r="B97" s="61" t="s">
         <v>155</v>
       </c>
@@ -6808,7 +6808,7 @@
       <c r="S97" s="59"/>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A98" s="179"/>
+      <c r="A98" s="180"/>
       <c r="B98" s="10" t="s">
         <v>157</v>
       </c>
@@ -6845,7 +6845,7 @@
       <c r="S98" s="8"/>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A99" s="179"/>
+      <c r="A99" s="180"/>
       <c r="B99" s="61" t="s">
         <v>159</v>
       </c>
@@ -6882,7 +6882,7 @@
       <c r="S99" s="59"/>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A100" s="179"/>
+      <c r="A100" s="180"/>
       <c r="B100" s="61" t="s">
         <v>161</v>
       </c>
@@ -6917,7 +6917,7 @@
       <c r="S100" s="59"/>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A101" s="179"/>
+      <c r="A101" s="180"/>
       <c r="B101" s="61" t="s">
         <v>163</v>
       </c>
@@ -6952,7 +6952,7 @@
       <c r="S101" s="59"/>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A102" s="179"/>
+      <c r="A102" s="180"/>
       <c r="B102" s="10" t="s">
         <v>165</v>
       </c>
@@ -6986,7 +6986,7 @@
       <c r="S102" s="8"/>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A103" s="192"/>
+      <c r="A103" s="193"/>
       <c r="B103" s="65" t="s">
         <v>167</v>
       </c>
@@ -7021,7 +7021,7 @@
       <c r="S103" s="87"/>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A104" s="178" t="s">
+      <c r="A104" s="179" t="s">
         <v>291</v>
       </c>
       <c r="B104" s="54" t="s">
@@ -7058,7 +7058,7 @@
       <c r="S104" s="59"/>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A105" s="179"/>
+      <c r="A105" s="180"/>
       <c r="B105" s="61" t="s">
         <v>171</v>
       </c>
@@ -7093,7 +7093,7 @@
       <c r="S105" s="59"/>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A106" s="179"/>
+      <c r="A106" s="180"/>
       <c r="B106" s="10" t="s">
         <v>173</v>
       </c>
@@ -7128,7 +7128,7 @@
       <c r="S106" s="8"/>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A107" s="179"/>
+      <c r="A107" s="180"/>
       <c r="B107" s="61" t="s">
         <v>175</v>
       </c>
@@ -7163,7 +7163,7 @@
       <c r="S107" s="59"/>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A108" s="179"/>
+      <c r="A108" s="180"/>
       <c r="B108" s="61" t="s">
         <v>177</v>
       </c>
@@ -7198,7 +7198,7 @@
       <c r="S108" s="59"/>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A109" s="179"/>
+      <c r="A109" s="180"/>
       <c r="B109" s="61" t="s">
         <v>179</v>
       </c>
@@ -7233,7 +7233,7 @@
       <c r="S109" s="59"/>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A110" s="179"/>
+      <c r="A110" s="180"/>
       <c r="B110" s="10" t="s">
         <v>181</v>
       </c>
@@ -7268,7 +7268,7 @@
       <c r="S110" s="8"/>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A111" s="179"/>
+      <c r="A111" s="180"/>
       <c r="B111" s="61" t="s">
         <v>183</v>
       </c>
@@ -7303,7 +7303,7 @@
       <c r="S111" s="59"/>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A112" s="179"/>
+      <c r="A112" s="180"/>
       <c r="B112" s="61" t="s">
         <v>185</v>
       </c>
@@ -7338,7 +7338,7 @@
       <c r="S112" s="59"/>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A113" s="179"/>
+      <c r="A113" s="180"/>
       <c r="B113" s="61" t="s">
         <v>187</v>
       </c>
@@ -7373,7 +7373,7 @@
       <c r="S113" s="59"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A114" s="179"/>
+      <c r="A114" s="180"/>
       <c r="B114" s="10" t="s">
         <v>189</v>
       </c>
@@ -7408,7 +7408,7 @@
       <c r="S114" s="8"/>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A115" s="179"/>
+      <c r="A115" s="180"/>
       <c r="B115" s="61" t="s">
         <v>191</v>
       </c>
@@ -7443,7 +7443,7 @@
       <c r="S115" s="59"/>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A116" s="179"/>
+      <c r="A116" s="180"/>
       <c r="B116" s="61" t="s">
         <v>231</v>
       </c>
@@ -7478,7 +7478,7 @@
       <c r="S116" s="59"/>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A117" s="179"/>
+      <c r="A117" s="180"/>
       <c r="B117" s="61" t="s">
         <v>193</v>
       </c>
@@ -7513,7 +7513,7 @@
       <c r="S117" s="59"/>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A118" s="179"/>
+      <c r="A118" s="180"/>
       <c r="B118" s="10" t="s">
         <v>229</v>
       </c>
@@ -7547,7 +7547,7 @@
       <c r="S118" s="8"/>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A119" s="192"/>
+      <c r="A119" s="193"/>
       <c r="B119" s="65" t="s">
         <v>195</v>
       </c>
@@ -7582,7 +7582,7 @@
       <c r="S119" s="87"/>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A120" s="178" t="s">
+      <c r="A120" s="179" t="s">
         <v>7</v>
       </c>
       <c r="B120" s="54" t="s">
@@ -7619,7 +7619,7 @@
       <c r="S120" s="59"/>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A121" s="179"/>
+      <c r="A121" s="180"/>
       <c r="B121" s="61" t="s">
         <v>227</v>
       </c>
@@ -7654,7 +7654,7 @@
       <c r="S121" s="59"/>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A122" s="179"/>
+      <c r="A122" s="180"/>
       <c r="B122" s="10" t="s">
         <v>199</v>
       </c>
@@ -7689,7 +7689,7 @@
       <c r="S122" s="8"/>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A123" s="179"/>
+      <c r="A123" s="180"/>
       <c r="B123" s="61" t="s">
         <v>223</v>
       </c>
@@ -7724,7 +7724,7 @@
       <c r="S123" s="59"/>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A124" s="179"/>
+      <c r="A124" s="180"/>
       <c r="B124" s="61" t="s">
         <v>225</v>
       </c>
@@ -7759,7 +7759,7 @@
       <c r="S124" s="59"/>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A125" s="179"/>
+      <c r="A125" s="180"/>
       <c r="B125" s="61" t="s">
         <v>201</v>
       </c>
@@ -7794,7 +7794,7 @@
       <c r="S125" s="59"/>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A126" s="179"/>
+      <c r="A126" s="180"/>
       <c r="B126" s="10" t="s">
         <v>203</v>
       </c>
@@ -7829,7 +7829,7 @@
       <c r="S126" s="8"/>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A127" s="179"/>
+      <c r="A127" s="180"/>
       <c r="B127" s="61" t="s">
         <v>205</v>
       </c>
@@ -7864,7 +7864,7 @@
       <c r="S127" s="59"/>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A128" s="179"/>
+      <c r="A128" s="180"/>
       <c r="B128" s="61" t="s">
         <v>207</v>
       </c>
@@ -7899,7 +7899,7 @@
       <c r="S128" s="59"/>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A129" s="179"/>
+      <c r="A129" s="180"/>
       <c r="B129" s="61" t="s">
         <v>209</v>
       </c>
@@ -7934,7 +7934,7 @@
       <c r="S129" s="59"/>
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A130" s="179"/>
+      <c r="A130" s="180"/>
       <c r="B130" s="10" t="s">
         <v>211</v>
       </c>
@@ -7969,7 +7969,7 @@
       <c r="S130" s="8"/>
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A131" s="179"/>
+      <c r="A131" s="180"/>
       <c r="B131" s="61" t="s">
         <v>213</v>
       </c>
@@ -8004,7 +8004,7 @@
       <c r="S131" s="59"/>
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A132" s="179"/>
+      <c r="A132" s="180"/>
       <c r="B132" s="61" t="s">
         <v>215</v>
       </c>
@@ -8039,7 +8039,7 @@
       <c r="S132" s="59"/>
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A133" s="179"/>
+      <c r="A133" s="180"/>
       <c r="B133" s="61" t="s">
         <v>217</v>
       </c>
@@ -8074,7 +8074,7 @@
       <c r="S133" s="59"/>
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A134" s="179"/>
+      <c r="A134" s="180"/>
       <c r="B134" s="10" t="s">
         <v>219</v>
       </c>
@@ -8105,7 +8105,7 @@
       <c r="S134" s="8"/>
     </row>
     <row r="135" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="180"/>
+      <c r="A135" s="181"/>
       <c r="B135" s="70" t="s">
         <v>221</v>
       </c>
@@ -8168,33 +8168,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId4" name="Control 3">
+        <control shapeId="1025" r:id="rId4" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId4" name="Control 3"/>
+        <control shapeId="1025" r:id="rId4" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1026" r:id="rId6" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId5">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
@@ -8218,27 +8218,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId7" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId8">
+        <control shapeId="1027" r:id="rId8" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId7" name="Control 1"/>
+        <control shapeId="1027" r:id="rId8" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9070,8 +9070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:A42"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9449,8 +9449,8 @@
       </c>
     </row>
     <row r="7" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="148" t="s">
-        <v>16</v>
+      <c r="A7" s="178" t="s">
+        <v>17</v>
       </c>
       <c r="B7" s="149" t="s">
         <v>399</v>
@@ -9508,8 +9508,8 @@
       </c>
     </row>
     <row r="8" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="148" t="s">
-        <v>16</v>
+      <c r="A8" s="178" t="s">
+        <v>17</v>
       </c>
       <c r="B8" s="149" t="s">
         <v>399</v>
@@ -9567,8 +9567,8 @@
       </c>
     </row>
     <row r="9" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="148" t="s">
-        <v>16</v>
+      <c r="A9" s="178" t="s">
+        <v>17</v>
       </c>
       <c r="B9" s="149" t="s">
         <v>399</v>
@@ -10511,7 +10511,7 @@
       </c>
     </row>
     <row r="25" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="196" t="s">
+      <c r="A25" s="178" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="173" t="s">
@@ -10688,7 +10688,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="196" t="s">
+      <c r="A28" s="178" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="173" t="s">
@@ -10747,7 +10747,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="196" t="s">
+      <c r="A29" s="178" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="173" t="s">
@@ -10806,7 +10806,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="196" t="s">
+      <c r="A30" s="178" t="s">
         <v>17</v>
       </c>
       <c r="B30" s="173" t="s">
@@ -10865,7 +10865,7 @@
       </c>
     </row>
     <row r="31" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="196" t="s">
+      <c r="A31" s="178" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="173" t="s">
@@ -11101,7 +11101,7 @@
       </c>
     </row>
     <row r="35" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="196" t="s">
+      <c r="A35" s="178" t="s">
         <v>17</v>
       </c>
       <c r="B35" s="173" t="s">
@@ -11278,7 +11278,7 @@
       </c>
     </row>
     <row r="38" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="196" t="s">
+      <c r="A38" s="178" t="s">
         <v>17</v>
       </c>
       <c r="B38" s="173" t="s">
@@ -11337,7 +11337,7 @@
       </c>
     </row>
     <row r="39" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="196" t="s">
+      <c r="A39" s="178" t="s">
         <v>17</v>
       </c>
       <c r="B39" s="173" t="s">
@@ -11455,7 +11455,7 @@
       </c>
     </row>
     <row r="41" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="196" t="s">
+      <c r="A41" s="178" t="s">
         <v>17</v>
       </c>
       <c r="B41" s="173" t="s">
@@ -11514,7 +11514,7 @@
       </c>
     </row>
     <row r="42" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="196" t="s">
+      <c r="A42" s="178" t="s">
         <v>17</v>
       </c>
       <c r="B42" s="173" t="s">
@@ -11632,8 +11632,8 @@
       </c>
     </row>
     <row r="44" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="148" t="s">
-        <v>16</v>
+      <c r="A44" s="178" t="s">
+        <v>17</v>
       </c>
       <c r="B44" s="173" t="s">
         <v>401</v>

</xml_diff>

<commit_message>
Removed         WaitUtils.waitForElementToBeVisible and replaced with normal selenium timeouts
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/DevicesData.xlsx
+++ b/src/test/resources/configs/data/excel/DevicesData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9455" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9417" uniqueCount="614">
   <si>
     <t>GMD (C-Y)</t>
   </si>
@@ -3174,7 +3174,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8166,33 +8166,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="Control 1">
+        <control shapeId="1027" r:id="rId4" name="Control 3">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+        <control shapeId="1027" r:id="rId4" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1026" r:id="rId6" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId7">
+          <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
@@ -8216,27 +8216,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId8" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId7">
+        <control shapeId="1025" r:id="rId7" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId8" name="Control 3"/>
+        <control shapeId="1025" r:id="rId7" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9023,10 +9023,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9222,35 +9222,35 @@
       <c r="A4" s="148" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="173" t="s">
-        <v>399</v>
-      </c>
-      <c r="C4" s="147" t="s">
-        <v>288</v>
+      <c r="B4" s="145" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="149" t="s">
+        <v>431</v>
       </c>
       <c r="D4" s="143" t="s">
-        <v>280</v>
+        <v>77</v>
       </c>
       <c r="E4" s="143" t="s">
-        <v>463</v>
+        <v>78</v>
       </c>
       <c r="F4" s="149" t="s">
         <v>431</v>
       </c>
-      <c r="G4" s="149" t="s">
-        <v>431</v>
+      <c r="G4" s="152" t="s">
+        <v>16</v>
       </c>
       <c r="H4" s="149" t="s">
         <v>431</v>
       </c>
       <c r="I4" s="149" t="s">
-        <v>17</v>
+        <v>431</v>
       </c>
       <c r="J4" s="149" t="s">
-        <v>17</v>
+        <v>431</v>
       </c>
       <c r="K4" s="149" t="s">
-        <v>17</v>
+        <v>431</v>
       </c>
       <c r="L4" s="149" t="s">
         <v>431</v>
@@ -9258,49 +9258,49 @@
       <c r="M4" s="149" t="s">
         <v>431</v>
       </c>
-      <c r="N4" s="148" t="s">
-        <v>294</v>
-      </c>
-      <c r="O4" s="148" t="s">
-        <v>613</v>
+      <c r="N4" s="149" t="s">
+        <v>431</v>
+      </c>
+      <c r="O4" s="149" t="s">
+        <v>431</v>
       </c>
       <c r="P4" s="149" t="s">
         <v>431</v>
       </c>
-      <c r="Q4" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="R4" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="S4" s="149" t="s">
-        <v>431</v>
+      <c r="Q4" s="148" t="s">
+        <v>385</v>
+      </c>
+      <c r="R4" s="148" t="s">
+        <v>386</v>
+      </c>
+      <c r="S4" s="148" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="148" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="145" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="149" t="s">
-        <v>431</v>
+      <c r="A5" s="146" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="147" t="s">
+        <v>413</v>
+      </c>
+      <c r="C5" s="147" t="s">
+        <v>4</v>
       </c>
       <c r="D5" s="143" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E5" s="143" t="s">
-        <v>78</v>
+        <v>496</v>
       </c>
       <c r="F5" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="G5" s="152" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="G5" s="172" t="s">
+        <v>17</v>
       </c>
       <c r="H5" s="149" t="s">
-        <v>431</v>
+        <v>16</v>
       </c>
       <c r="I5" s="149" t="s">
         <v>431</v>
@@ -9312,13 +9312,13 @@
         <v>431</v>
       </c>
       <c r="L5" s="149" t="s">
-        <v>431</v>
+        <v>17</v>
       </c>
       <c r="M5" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="N5" s="149" t="s">
-        <v>431</v>
+        <v>16</v>
+      </c>
+      <c r="N5" s="148" t="s">
+        <v>296</v>
       </c>
       <c r="O5" s="149" t="s">
         <v>431</v>
@@ -9326,40 +9326,40 @@
       <c r="P5" s="149" t="s">
         <v>431</v>
       </c>
-      <c r="Q5" s="148" t="s">
-        <v>385</v>
-      </c>
-      <c r="R5" s="148" t="s">
-        <v>386</v>
-      </c>
-      <c r="S5" s="148" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="146" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="147" t="s">
-        <v>413</v>
-      </c>
-      <c r="C6" s="147" t="s">
-        <v>4</v>
+      <c r="Q5" s="149" t="s">
+        <v>431</v>
+      </c>
+      <c r="R5" s="149" t="s">
+        <v>431</v>
+      </c>
+      <c r="S5" s="149" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" s="148" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="148" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="149" t="s">
+        <v>397</v>
+      </c>
+      <c r="C6" s="149" t="s">
+        <v>431</v>
       </c>
       <c r="D6" s="143" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="E6" s="143" t="s">
-        <v>496</v>
-      </c>
-      <c r="F6" s="149" t="s">
+        <v>432</v>
+      </c>
+      <c r="F6" s="172" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="172" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="149" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H6" s="172" t="s">
+        <v>17</v>
       </c>
       <c r="I6" s="149" t="s">
         <v>431</v>
@@ -9371,13 +9371,13 @@
         <v>431</v>
       </c>
       <c r="L6" s="149" t="s">
-        <v>17</v>
+        <v>431</v>
       </c>
       <c r="M6" s="149" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="148" t="s">
-        <v>296</v>
+        <v>431</v>
+      </c>
+      <c r="N6" s="149" t="s">
+        <v>431</v>
       </c>
       <c r="O6" s="149" t="s">
         <v>431</v>
@@ -9392,124 +9392,6 @@
         <v>431</v>
       </c>
       <c r="S6" s="149" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="146" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="147" t="s">
-        <v>413</v>
-      </c>
-      <c r="C7" s="147" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="143" t="s">
-        <v>500</v>
-      </c>
-      <c r="E7" s="143" t="s">
-        <v>501</v>
-      </c>
-      <c r="F7" s="149" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="172" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="149" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="J7" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="K7" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="L7" s="149" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="149" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" s="148" t="s">
-        <v>296</v>
-      </c>
-      <c r="O7" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="P7" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="Q7" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="R7" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="S7" s="149" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" s="148" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="148" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="149" t="s">
-        <v>397</v>
-      </c>
-      <c r="C8" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="D8" s="143" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="143" t="s">
-        <v>432</v>
-      </c>
-      <c r="F8" s="172" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="172" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="172" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="J8" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="K8" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="L8" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="M8" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="N8" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="O8" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="P8" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="Q8" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="R8" s="149" t="s">
-        <v>431</v>
-      </c>
-      <c r="S8" s="149" t="s">
         <v>431</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Try and add multiple devices for smoke tests
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/DevicesData.xlsx
+++ b/src/test/resources/configs/data/excel/DevicesData.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10695" windowHeight="9375" tabRatio="485" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10695" windowHeight="9375" tabRatio="485" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="1" r:id="rId1"/>
     <sheet name="Calculations" sheetId="2" r:id="rId2"/>
-    <sheet name="TestDataWellFormed_Simple" sheetId="7" r:id="rId3"/>
-    <sheet name="TestDataWellFormed_Simple_" sheetId="5" r:id="rId4"/>
+    <sheet name="TestDataWellFormed_Simple_4Line" sheetId="7" r:id="rId3"/>
+    <sheet name="TestDataWellFormed_Simple" sheetId="5" r:id="rId4"/>
     <sheet name="TestDataWellFormed" sheetId="4" r:id="rId5"/>
     <sheet name="TestDataWellFormed_Simple_COPY" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TestDataWellFormed_Simple_!$A$1:$S$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TestDataWellFormed_Simple!$A$1:$S$136</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -3174,7 +3174,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8166,33 +8166,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId4" name="Control 3">
+        <control shapeId="1025" r:id="rId4" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId4" name="Control 3"/>
+        <control shapeId="1025" r:id="rId4" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1026" r:id="rId6" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId5">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
@@ -8216,27 +8216,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId7" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId8">
+        <control shapeId="1027" r:id="rId8" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId7" name="Control 1"/>
+        <control shapeId="1027" r:id="rId8" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9025,8 +9025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9404,7 +9404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S146"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Renamed excel data sheet _full
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/DevicesData.xlsx
+++ b/src/test/resources/configs/data/excel/DevicesData.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10695" windowHeight="9375" tabRatio="485" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10695" windowHeight="9375" tabRatio="485" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="1" r:id="rId1"/>
     <sheet name="Calculations" sheetId="2" r:id="rId2"/>
-    <sheet name="TestDataWellFormed_Simple_4Line" sheetId="7" r:id="rId3"/>
-    <sheet name="TestDataWellFormed_Simple" sheetId="5" r:id="rId4"/>
+    <sheet name="TestDataWellFormed_Simple" sheetId="7" r:id="rId3"/>
+    <sheet name="TestDataWellFormed_Simple_full" sheetId="5" r:id="rId4"/>
     <sheet name="TestDataWellFormed" sheetId="4" r:id="rId5"/>
     <sheet name="TestDataWellFormed_Simple_COPY" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TestDataWellFormed_Simple!$A$1:$S$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TestDataWellFormed_Simple_full!$A$1:$S$136</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -9026,7 +9026,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added code to add multiple devices
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/DevicesData.xlsx
+++ b/src/test/resources/configs/data/excel/DevicesData.xlsx
@@ -9404,8 +9404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C152" sqref="C152"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="A134" sqref="A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9489,7 +9489,7 @@
     </row>
     <row r="2" spans="1:19" s="148" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="149" t="s">
         <v>397</v>
@@ -9548,7 +9548,7 @@
     </row>
     <row r="3" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="149" t="s">
         <v>397</v>
@@ -9607,7 +9607,7 @@
     </row>
     <row r="4" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="149" t="s">
         <v>397</v>
@@ -9666,7 +9666,7 @@
     </row>
     <row r="5" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="149" t="s">
         <v>397</v>
@@ -9784,7 +9784,7 @@
     </row>
     <row r="7" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="149" t="s">
         <v>397</v>
@@ -9843,7 +9843,7 @@
     </row>
     <row r="8" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="149" t="s">
         <v>397</v>
@@ -9902,7 +9902,7 @@
     </row>
     <row r="9" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="149" t="s">
         <v>397</v>
@@ -10020,7 +10020,7 @@
     </row>
     <row r="11" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="149" t="s">
         <v>397</v>
@@ -10079,7 +10079,7 @@
     </row>
     <row r="12" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="149" t="s">
         <v>397</v>
@@ -10138,7 +10138,7 @@
     </row>
     <row r="13" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="149" t="s">
         <v>397</v>
@@ -10197,7 +10197,7 @@
     </row>
     <row r="14" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="149" t="s">
         <v>397</v>
@@ -10256,7 +10256,7 @@
     </row>
     <row r="15" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="149" t="s">
         <v>397</v>
@@ -10315,7 +10315,7 @@
     </row>
     <row r="16" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="149" t="s">
         <v>397</v>
@@ -10374,7 +10374,7 @@
     </row>
     <row r="17" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="149" t="s">
         <v>397</v>
@@ -10433,7 +10433,7 @@
     </row>
     <row r="18" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="149" t="s">
         <v>397</v>
@@ -10492,7 +10492,7 @@
     </row>
     <row r="19" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="149" t="s">
         <v>397</v>
@@ -10551,7 +10551,7 @@
     </row>
     <row r="20" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="149" t="s">
         <v>397</v>
@@ -10610,7 +10610,7 @@
     </row>
     <row r="21" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="149" t="s">
         <v>397</v>
@@ -10669,7 +10669,7 @@
     </row>
     <row r="22" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="149" t="s">
         <v>397</v>
@@ -10846,7 +10846,7 @@
     </row>
     <row r="25" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="173" t="s">
         <v>399</v>
@@ -10905,7 +10905,7 @@
     </row>
     <row r="26" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="173" t="s">
         <v>399</v>
@@ -10964,7 +10964,7 @@
     </row>
     <row r="27" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="173" t="s">
         <v>399</v>
@@ -11023,7 +11023,7 @@
     </row>
     <row r="28" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="173" t="s">
         <v>399</v>
@@ -11082,7 +11082,7 @@
     </row>
     <row r="29" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="173" t="s">
         <v>399</v>
@@ -11141,7 +11141,7 @@
     </row>
     <row r="30" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" s="173" t="s">
         <v>399</v>
@@ -11200,7 +11200,7 @@
     </row>
     <row r="31" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" s="173" t="s">
         <v>399</v>
@@ -11259,7 +11259,7 @@
     </row>
     <row r="32" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" s="173" t="s">
         <v>399</v>
@@ -11318,7 +11318,7 @@
     </row>
     <row r="33" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="173" t="s">
         <v>399</v>
@@ -11377,7 +11377,7 @@
     </row>
     <row r="34" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="173" t="s">
         <v>399</v>
@@ -11436,7 +11436,7 @@
     </row>
     <row r="35" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" s="173" t="s">
         <v>399</v>
@@ -11495,7 +11495,7 @@
     </row>
     <row r="36" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" s="173" t="s">
         <v>399</v>
@@ -11554,7 +11554,7 @@
     </row>
     <row r="37" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37" s="173" t="s">
         <v>399</v>
@@ -11613,7 +11613,7 @@
     </row>
     <row r="38" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38" s="173" t="s">
         <v>399</v>
@@ -11672,7 +11672,7 @@
     </row>
     <row r="39" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B39" s="173" t="s">
         <v>399</v>
@@ -11731,7 +11731,7 @@
     </row>
     <row r="40" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B40" s="173" t="s">
         <v>399</v>
@@ -11790,7 +11790,7 @@
     </row>
     <row r="41" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B41" s="173" t="s">
         <v>399</v>
@@ -11849,7 +11849,7 @@
     </row>
     <row r="42" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B42" s="173" t="s">
         <v>399</v>
@@ -11908,7 +11908,7 @@
     </row>
     <row r="43" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43" s="173" t="s">
         <v>399</v>
@@ -11967,7 +11967,7 @@
     </row>
     <row r="44" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B44" s="173" t="s">
         <v>399</v>
@@ -12026,7 +12026,7 @@
     </row>
     <row r="45" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B45" s="173" t="s">
         <v>399</v>
@@ -12085,7 +12085,7 @@
     </row>
     <row r="46" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B46" s="173" t="s">
         <v>399</v>
@@ -12262,7 +12262,7 @@
     </row>
     <row r="49" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B49" s="149" t="s">
         <v>399</v>
@@ -12439,7 +12439,7 @@
     </row>
     <row r="52" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B52" s="145" t="s">
         <v>22</v>
@@ -12557,7 +12557,7 @@
     </row>
     <row r="54" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B54" s="147" t="s">
         <v>413</v>
@@ -12616,7 +12616,7 @@
     </row>
     <row r="55" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B55" s="147" t="s">
         <v>413</v>
@@ -12675,7 +12675,7 @@
     </row>
     <row r="56" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B56" s="147" t="s">
         <v>413</v>
@@ -12734,7 +12734,7 @@
     </row>
     <row r="57" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B57" s="147" t="s">
         <v>413</v>
@@ -12793,7 +12793,7 @@
     </row>
     <row r="58" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B58" s="147" t="s">
         <v>413</v>
@@ -12852,7 +12852,7 @@
     </row>
     <row r="59" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B59" s="147" t="s">
         <v>413</v>
@@ -12911,7 +12911,7 @@
     </row>
     <row r="60" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B60" s="147" t="s">
         <v>413</v>
@@ -12970,7 +12970,7 @@
     </row>
     <row r="61" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B61" s="147" t="s">
         <v>413</v>
@@ -13029,7 +13029,7 @@
     </row>
     <row r="62" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B62" s="147" t="s">
         <v>413</v>
@@ -13088,7 +13088,7 @@
     </row>
     <row r="63" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B63" s="147" t="s">
         <v>413</v>
@@ -13147,7 +13147,7 @@
     </row>
     <row r="64" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B64" s="147" t="s">
         <v>413</v>
@@ -13206,7 +13206,7 @@
     </row>
     <row r="65" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B65" s="147" t="s">
         <v>413</v>
@@ -13265,7 +13265,7 @@
     </row>
     <row r="66" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B66" s="147" t="s">
         <v>413</v>
@@ -13324,7 +13324,7 @@
     </row>
     <row r="67" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B67" s="147" t="s">
         <v>413</v>
@@ -13383,7 +13383,7 @@
     </row>
     <row r="68" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B68" s="147" t="s">
         <v>413</v>
@@ -13442,7 +13442,7 @@
     </row>
     <row r="69" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B69" s="147" t="s">
         <v>413</v>
@@ -13560,7 +13560,7 @@
     </row>
     <row r="71" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B71" s="147" t="s">
         <v>413</v>
@@ -13619,7 +13619,7 @@
     </row>
     <row r="72" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B72" s="147" t="s">
         <v>413</v>
@@ -13737,7 +13737,7 @@
     </row>
     <row r="74" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B74" s="147" t="s">
         <v>413</v>
@@ -13796,7 +13796,7 @@
     </row>
     <row r="75" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B75" s="147" t="s">
         <v>413</v>
@@ -13855,7 +13855,7 @@
     </row>
     <row r="76" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B76" s="147" t="s">
         <v>413</v>
@@ -13973,7 +13973,7 @@
     </row>
     <row r="78" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B78" s="147" t="s">
         <v>413</v>
@@ -14032,7 +14032,7 @@
     </row>
     <row r="79" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B79" s="147" t="s">
         <v>413</v>
@@ -14091,7 +14091,7 @@
     </row>
     <row r="80" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B80" s="147" t="s">
         <v>413</v>
@@ -14150,7 +14150,7 @@
     </row>
     <row r="81" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B81" s="147" t="s">
         <v>413</v>
@@ -14209,7 +14209,7 @@
     </row>
     <row r="82" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B82" s="147" t="s">
         <v>413</v>
@@ -14268,7 +14268,7 @@
     </row>
     <row r="83" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B83" s="147" t="s">
         <v>413</v>
@@ -14327,7 +14327,7 @@
     </row>
     <row r="84" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B84" s="147" t="s">
         <v>413</v>
@@ -14386,7 +14386,7 @@
     </row>
     <row r="85" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B85" s="147" t="s">
         <v>413</v>
@@ -14445,7 +14445,7 @@
     </row>
     <row r="86" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B86" s="147" t="s">
         <v>413</v>
@@ -14504,7 +14504,7 @@
     </row>
     <row r="87" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B87" s="147" t="s">
         <v>413</v>
@@ -14563,7 +14563,7 @@
     </row>
     <row r="88" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B88" s="147" t="s">
         <v>413</v>
@@ -14622,7 +14622,7 @@
     </row>
     <row r="89" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B89" s="147" t="s">
         <v>413</v>
@@ -14681,7 +14681,7 @@
     </row>
     <row r="90" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B90" s="147" t="s">
         <v>413</v>
@@ -14740,7 +14740,7 @@
     </row>
     <row r="91" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B91" s="147" t="s">
         <v>413</v>
@@ -14799,7 +14799,7 @@
     </row>
     <row r="92" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B92" s="147" t="s">
         <v>413</v>
@@ -14858,7 +14858,7 @@
     </row>
     <row r="93" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B93" s="147" t="s">
         <v>413</v>
@@ -14917,7 +14917,7 @@
     </row>
     <row r="94" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B94" s="147" t="s">
         <v>413</v>
@@ -14976,7 +14976,7 @@
     </row>
     <row r="95" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B95" s="147" t="s">
         <v>413</v>
@@ -15035,7 +15035,7 @@
     </row>
     <row r="96" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B96" s="147" t="s">
         <v>413</v>
@@ -15094,7 +15094,7 @@
     </row>
     <row r="97" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B97" s="147" t="s">
         <v>413</v>
@@ -15153,7 +15153,7 @@
     </row>
     <row r="98" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B98" s="147" t="s">
         <v>413</v>
@@ -15212,7 +15212,7 @@
     </row>
     <row r="99" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B99" s="147" t="s">
         <v>413</v>
@@ -15271,7 +15271,7 @@
     </row>
     <row r="100" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B100" s="147" t="s">
         <v>413</v>
@@ -15330,7 +15330,7 @@
     </row>
     <row r="101" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B101" s="147" t="s">
         <v>413</v>
@@ -15389,7 +15389,7 @@
     </row>
     <row r="102" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B102" s="147" t="s">
         <v>413</v>
@@ -15448,7 +15448,7 @@
     </row>
     <row r="103" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B103" s="147" t="s">
         <v>413</v>
@@ -15507,7 +15507,7 @@
     </row>
     <row r="104" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B104" s="147" t="s">
         <v>413</v>
@@ -15566,7 +15566,7 @@
     </row>
     <row r="105" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B105" s="147" t="s">
         <v>413</v>
@@ -15625,7 +15625,7 @@
     </row>
     <row r="106" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B106" s="147" t="s">
         <v>413</v>
@@ -15684,7 +15684,7 @@
     </row>
     <row r="107" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B107" s="147" t="s">
         <v>413</v>
@@ -15743,7 +15743,7 @@
     </row>
     <row r="108" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B108" s="147" t="s">
         <v>413</v>
@@ -15802,7 +15802,7 @@
     </row>
     <row r="109" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B109" s="147" t="s">
         <v>413</v>
@@ -15861,7 +15861,7 @@
     </row>
     <row r="110" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B110" s="147" t="s">
         <v>413</v>
@@ -15920,7 +15920,7 @@
     </row>
     <row r="111" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B111" s="147" t="s">
         <v>413</v>
@@ -15979,7 +15979,7 @@
     </row>
     <row r="112" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B112" s="147" t="s">
         <v>413</v>
@@ -16038,7 +16038,7 @@
     </row>
     <row r="113" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B113" s="147" t="s">
         <v>413</v>
@@ -16097,7 +16097,7 @@
     </row>
     <row r="114" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B114" s="147" t="s">
         <v>413</v>
@@ -16156,7 +16156,7 @@
     </row>
     <row r="115" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B115" s="147" t="s">
         <v>413</v>
@@ -16215,7 +16215,7 @@
     </row>
     <row r="116" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B116" s="147" t="s">
         <v>413</v>
@@ -16274,7 +16274,7 @@
     </row>
     <row r="117" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B117" s="147" t="s">
         <v>413</v>
@@ -16333,7 +16333,7 @@
     </row>
     <row r="118" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B118" s="147" t="s">
         <v>413</v>
@@ -16392,7 +16392,7 @@
     </row>
     <row r="119" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B119" s="147" t="s">
         <v>413</v>
@@ -16451,7 +16451,7 @@
     </row>
     <row r="120" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B120" s="147" t="s">
         <v>413</v>
@@ -16510,7 +16510,7 @@
     </row>
     <row r="121" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B121" s="147" t="s">
         <v>413</v>
@@ -16569,7 +16569,7 @@
     </row>
     <row r="122" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B122" s="147" t="s">
         <v>413</v>
@@ -16628,7 +16628,7 @@
     </row>
     <row r="123" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B123" s="147" t="s">
         <v>413</v>
@@ -16687,7 +16687,7 @@
     </row>
     <row r="124" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B124" s="147" t="s">
         <v>413</v>
@@ -16746,7 +16746,7 @@
     </row>
     <row r="125" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B125" s="147" t="s">
         <v>413</v>
@@ -16805,7 +16805,7 @@
     </row>
     <row r="126" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B126" s="147" t="s">
         <v>413</v>
@@ -16864,7 +16864,7 @@
     </row>
     <row r="127" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B127" s="147" t="s">
         <v>413</v>
@@ -16923,7 +16923,7 @@
     </row>
     <row r="128" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B128" s="147" t="s">
         <v>413</v>
@@ -16982,7 +16982,7 @@
     </row>
     <row r="129" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B129" s="147" t="s">
         <v>413</v>
@@ -17041,7 +17041,7 @@
     </row>
     <row r="130" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B130" s="147" t="s">
         <v>413</v>
@@ -17100,7 +17100,7 @@
     </row>
     <row r="131" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B131" s="147" t="s">
         <v>413</v>
@@ -17159,7 +17159,7 @@
     </row>
     <row r="132" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B132" s="147" t="s">
         <v>413</v>
@@ -17218,7 +17218,7 @@
     </row>
     <row r="133" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B133" s="147" t="s">
         <v>413</v>
@@ -17277,7 +17277,7 @@
     </row>
     <row r="134" spans="1:19" s="148" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B134" s="147" t="s">
         <v>413</v>
@@ -17507,7 +17507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y146"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>

</xml_diff>